<commit_message>
MAJ timecodes et commentaires pour montage
</commit_message>
<xml_diff>
--- a/Recap.xlsx
+++ b/Recap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Nom du plan</t>
   </si>
@@ -82,15 +82,9 @@
     <t>Baissé-Relevé</t>
   </si>
   <si>
-    <t>Cerf qui humme</t>
-  </si>
-  <si>
     <t>Relève sur 2 pattes</t>
   </si>
   <si>
-    <t>Contre plongée torse</t>
-  </si>
-  <si>
     <t>Marche de face</t>
   </si>
   <si>
@@ -112,19 +106,28 @@
     <t>Rendu idéalement à refaire</t>
   </si>
   <si>
-    <t>Rendu en cours</t>
-  </si>
-  <si>
     <t>Scène à faire</t>
   </si>
   <si>
-    <t>Cadrage à faire</t>
-  </si>
-  <si>
-    <t>total=504</t>
-  </si>
-  <si>
     <t>Rendu idéalement à refaire avec chaise bug lumère plus basse</t>
+  </si>
+  <si>
+    <t>Cerf qui hume</t>
+  </si>
+  <si>
+    <t>Contre plongée</t>
+  </si>
+  <si>
+    <t>timecode fondu au noir: 2:22</t>
+  </si>
+  <si>
+    <t>Les times codes sont pas fixes. Privilégier la synchronisation arrivée de la deuxième araignée avec la 2'' mélodie de la boite à musique</t>
+  </si>
+  <si>
+    <t>(total es 3 précédents plans=504)</t>
+  </si>
+  <si>
+    <t>"/!\ à synchroniser le tic tac au mouvement du balancier"</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -170,12 +173,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -215,7 +212,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,7 +519,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,7 +530,7 @@
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="30.5703125" customWidth="1"/>
     <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -579,7 +575,7 @@
         <v>432</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -600,8 +596,11 @@
       <c r="E3" s="4">
         <v>96</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>30</v>
+      <c r="F3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -622,11 +621,11 @@
       <c r="E4" s="4">
         <v>408</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>30</v>
+      <c r="F4" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -647,11 +646,11 @@
       <c r="E5" s="4">
         <v>144</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>30</v>
+      <c r="F5" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -672,8 +671,8 @@
       <c r="E6" s="4">
         <v>144</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>31</v>
+      <c r="F6" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -695,7 +694,7 @@
         <v>144</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -717,7 +716,7 @@
         <v>120</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -739,7 +738,10 @@
         <v>144</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -760,8 +762,8 @@
       <c r="E10" s="4">
         <v>144</v>
       </c>
-      <c r="F10" s="10" t="s">
-        <v>36</v>
+      <c r="F10" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -783,7 +785,7 @@
         <v>144</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,7 +807,7 @@
         <v>120</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -826,8 +828,8 @@
       <c r="E13" s="4">
         <v>168</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>29</v>
+      <c r="F13" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -848,8 +850,8 @@
       <c r="E14" s="4">
         <v>72</v>
       </c>
-      <c r="F14" s="9" t="s">
-        <v>30</v>
+      <c r="F14" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -870,8 +872,8 @@
       <c r="E15" s="4">
         <v>192</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>32</v>
+      <c r="F15" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -892,13 +894,13 @@
       <c r="E16" s="4">
         <v>72</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2">
         <v>7.4305555555555555E-2</v>
@@ -914,13 +916,13 @@
       <c r="E17" s="4">
         <v>72</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>7.6388888888888895E-2</v>
@@ -936,13 +938,13 @@
       <c r="E18" s="4">
         <v>288</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3">
         <v>8.5300925925925919E-2</v>
@@ -959,12 +961,12 @@
         <v>144</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3">
         <v>8.9467592592592585E-2</v>
@@ -981,12 +983,12 @@
         <v>144</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2">
         <v>9.375E-2</v>
@@ -1002,12 +1004,15 @@
         <v>336</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>